<commit_message>
menambahkan implementasi CRUD pada database, menambahkan jam dan tanggal, menambahkan fitur alert ketika close aplikasi
</commit_message>
<xml_diff>
--- a/RAB ATK(1).xlsx
+++ b/RAB ATK(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f2e3f626e768742/Dokumen/Embarcadero/Studio/Projects/stock-barang-rudenim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{2C01C2C6-D1F5-401E-8B0D-FD468FA7981F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6320B5E3-A0CF-4438-A61A-4F84385FFDA5}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{2C01C2C6-D1F5-401E-8B0D-FD468FA7981F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAF9CD59-6D2A-4CCE-ABC5-F6E098A09CC5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{3074EB4E-354C-4093-BE8F-A625B48BC946}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="87">
   <si>
     <t>NO</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>Cutter</t>
+  </si>
+  <si>
+    <t>spidol</t>
   </si>
 </sst>
 </file>
@@ -349,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +377,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -510,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -526,6 +535,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -553,24 +580,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -889,7 +904,7 @@
   <dimension ref="A2:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -902,134 +917,138 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="22" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="20" t="s">
         <v>85</v>
       </c>
+      <c r="J2" s="30" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="16" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="28" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:12" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
-      <c r="B7" s="23">
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="1:12" s="13" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="12"/>
+      <c r="B7" s="14">
         <v>1</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="14">
         <v>6</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-    </row>
-    <row r="8" spans="1:12" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="23">
+      <c r="E7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:12" s="13" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="14">
         <v>2</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="14">
         <v>4</v>
       </c>
-      <c r="E8" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="5">
+      <c r="E8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:12" s="30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="12"/>
+      <c r="B9" s="31">
         <v>3</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="31">
         <v>2</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:12" s="22" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
-      <c r="B10" s="23">
+      <c r="E9" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+    </row>
+    <row r="10" spans="1:12" s="13" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="12"/>
+      <c r="B10" s="14">
         <v>4</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="14">
         <v>4</v>
       </c>
-      <c r="E10" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="E10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B11" s="5">
@@ -1112,39 +1131,41 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B16" s="5">
+    <row r="16" spans="1:12" s="30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
+      <c r="B16" s="31">
         <v>10</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="31">
         <v>1</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="5">
+      <c r="E16" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+    </row>
+    <row r="17" spans="1:7" s="30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="12"/>
+      <c r="B17" s="31">
         <v>11</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="31">
         <v>1</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E17" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B18" s="5">
         <v>12</v>
       </c>
@@ -1160,7 +1181,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B19" s="5">
         <v>13</v>
       </c>
@@ -1176,23 +1197,24 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="5">
-        <v>14</v>
-      </c>
-      <c r="C20" s="6" t="s">
+    <row r="20" spans="1:7" s="30" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="12"/>
+      <c r="B20" s="31">
+        <v>14</v>
+      </c>
+      <c r="C20" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="31">
         <v>2</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E20" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B21" s="5">
         <v>15</v>
       </c>
@@ -1208,7 +1230,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="5">
         <v>16</v>
       </c>
@@ -1224,7 +1246,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B23" s="5">
         <v>17</v>
       </c>
@@ -1240,7 +1262,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B24" s="5">
         <v>18</v>
       </c>
@@ -1256,7 +1278,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B25" s="5">
         <v>19</v>
       </c>
@@ -1272,7 +1294,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B26" s="5">
         <v>20</v>
       </c>
@@ -1288,7 +1310,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B27" s="5">
         <v>21</v>
       </c>
@@ -1304,7 +1326,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B28" s="5">
         <v>22</v>
       </c>
@@ -1320,7 +1342,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B29" s="5">
         <v>23</v>
       </c>
@@ -1336,7 +1358,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B30" s="5">
         <v>24</v>
       </c>
@@ -1352,7 +1374,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B31" s="5">
         <v>25</v>
       </c>
@@ -1368,7 +1390,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B32" s="5">
         <v>26</v>
       </c>
@@ -1480,39 +1502,39 @@
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:7" s="29" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="21"/>
-      <c r="B39" s="26">
+    <row r="39" spans="1:7" s="20" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="12"/>
+      <c r="B39" s="17">
         <v>33</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D39" s="26">
+      <c r="D39" s="17">
         <v>2</v>
       </c>
-      <c r="E39" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-    </row>
-    <row r="40" spans="1:7" s="29" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="21"/>
-      <c r="B40" s="26">
+      <c r="E39" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+    </row>
+    <row r="40" spans="1:7" s="20" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="12"/>
+      <c r="B40" s="17">
         <v>34</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D40" s="26">
+      <c r="D40" s="17">
         <v>2</v>
       </c>
-      <c r="E40" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
+      <c r="E40" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
     </row>
     <row r="41" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B41" s="5">
@@ -1706,37 +1728,37 @@
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B53" s="18">
+    <row r="53" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B53" s="9">
         <v>47</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D53" s="18">
+      <c r="D53" s="9">
         <v>10</v>
       </c>
-      <c r="E53" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-    </row>
-    <row r="54" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B54" s="18">
+      <c r="E53" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+    </row>
+    <row r="54" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B54" s="9">
         <v>48</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="18">
+      <c r="D54" s="9">
         <v>10</v>
       </c>
-      <c r="E54" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
+      <c r="E54" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
     </row>
     <row r="55" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B55" s="5">
@@ -1770,229 +1792,229 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B57" s="18">
+    <row r="57" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B57" s="9">
         <v>51</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D57" s="18">
+      <c r="D57" s="9">
         <v>10</v>
       </c>
-      <c r="E57" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-    </row>
-    <row r="58" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B58" s="18">
+      <c r="E57" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+    </row>
+    <row r="58" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B58" s="9">
         <v>52</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D58" s="18">
+      <c r="D58" s="9">
         <v>10</v>
       </c>
-      <c r="E58" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
-    </row>
-    <row r="59" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B59" s="18">
+      <c r="E58" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B59" s="9">
         <v>53</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D59" s="18">
+      <c r="D59" s="9">
         <v>10</v>
       </c>
-      <c r="E59" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-    </row>
-    <row r="60" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B60" s="18">
+      <c r="E59" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+    </row>
+    <row r="60" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B60" s="9">
         <v>54</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D60" s="18">
+      <c r="D60" s="9">
         <v>10</v>
       </c>
-      <c r="E60" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F60" s="20"/>
-      <c r="G60" s="20"/>
-    </row>
-    <row r="61" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B61" s="18">
+      <c r="E60" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+    </row>
+    <row r="61" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B61" s="9">
         <v>55</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D61" s="18">
+      <c r="D61" s="9">
         <v>5</v>
       </c>
-      <c r="E61" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F61" s="20"/>
-      <c r="G61" s="20"/>
-    </row>
-    <row r="62" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B62" s="18">
+      <c r="E61" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+    </row>
+    <row r="62" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B62" s="9">
         <v>56</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D62" s="18">
+      <c r="D62" s="9">
         <v>5</v>
       </c>
-      <c r="E62" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F62" s="20"/>
-      <c r="G62" s="20"/>
-    </row>
-    <row r="63" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B63" s="18">
+      <c r="E62" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+    </row>
+    <row r="63" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B63" s="9">
         <v>57</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D63" s="18">
+      <c r="D63" s="9">
         <v>5</v>
       </c>
-      <c r="E63" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F63" s="20"/>
-      <c r="G63" s="20"/>
-    </row>
-    <row r="64" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B64" s="18">
+      <c r="E63" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+    </row>
+    <row r="64" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B64" s="9">
         <v>58</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D64" s="18">
+      <c r="D64" s="9">
         <v>5</v>
       </c>
-      <c r="E64" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F64" s="20"/>
-      <c r="G64" s="20"/>
-    </row>
-    <row r="65" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B65" s="18">
+      <c r="E64" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+    </row>
+    <row r="65" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B65" s="9">
         <v>59</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D65" s="18">
+      <c r="D65" s="9">
         <v>5</v>
       </c>
-      <c r="E65" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F65" s="20"/>
-      <c r="G65" s="20"/>
-    </row>
-    <row r="66" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B66" s="18">
+      <c r="E65" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+    </row>
+    <row r="66" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B66" s="9">
         <v>60</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D66" s="18">
+      <c r="D66" s="9">
         <v>5</v>
       </c>
-      <c r="E66" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F66" s="20"/>
-      <c r="G66" s="20"/>
-    </row>
-    <row r="67" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B67" s="18">
+      <c r="E66" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+    </row>
+    <row r="67" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B67" s="9">
         <v>61</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="C67" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="18">
+      <c r="D67" s="9">
         <v>5</v>
       </c>
-      <c r="E67" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F67" s="20"/>
-      <c r="G67" s="20"/>
-    </row>
-    <row r="68" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B68" s="18">
+      <c r="E67" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+    </row>
+    <row r="68" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B68" s="9">
         <v>62</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="18">
+      <c r="D68" s="9">
         <v>5</v>
       </c>
-      <c r="E68" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F68" s="20"/>
-      <c r="G68" s="20"/>
-    </row>
-    <row r="69" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B69" s="18">
+      <c r="E68" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+    </row>
+    <row r="69" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B69" s="9">
         <v>63</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D69" s="18">
+      <c r="D69" s="9">
         <v>6</v>
       </c>
-      <c r="E69" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F69" s="20"/>
-      <c r="G69" s="20"/>
-    </row>
-    <row r="70" spans="2:7" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B70" s="18">
+      <c r="E69" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+    </row>
+    <row r="70" spans="2:7" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B70" s="9">
         <v>64</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="C70" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D70" s="18">
+      <c r="D70" s="9">
         <v>4</v>
       </c>
-      <c r="E70" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F70" s="20"/>
-      <c r="G70" s="20"/>
+      <c r="E70" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
     </row>
     <row r="71" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B71" s="5"/>
@@ -2003,13 +2025,13 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="15"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
       <c r="G72" s="3">
         <f>SUM(G7:G71)</f>
         <v>0</v>

</xml_diff>